<commit_message>
Test cases needing no test data to be run programically implemented
</commit_message>
<xml_diff>
--- a/Data_Driven/Resources/Excel_Files/Flight.xlsx
+++ b/Data_Driven/Resources/Excel_Files/Flight.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Test_Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Test_Case_List!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Test_Case_List!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="49">
   <si>
     <t>Run</t>
   </si>
@@ -29,36 +29,6 @@
     <t>Flight_Search_From</t>
   </si>
   <si>
-    <t>Test Type</t>
-  </si>
-  <si>
-    <t>TC_001</t>
-  </si>
-  <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>TC_005</t>
-  </si>
-  <si>
-    <t>TC_006</t>
-  </si>
-  <si>
-    <t>TC_007</t>
-  </si>
-  <si>
-    <t>TC_008</t>
-  </si>
-  <si>
-    <t>TC_009</t>
-  </si>
-  <si>
     <t>Verify Title</t>
   </si>
   <si>
@@ -92,12 +62,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t>Regression</t>
-  </si>
-  <si>
     <t>Flight_Search_To</t>
   </si>
   <si>
@@ -174,6 +138,33 @@
   </si>
   <si>
     <t>TC_015</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>TC_09</t>
   </si>
 </sst>
 </file>
@@ -629,343 +620,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="D15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="D16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F16"/>
+  <autoFilter ref="A1:E16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -995,7 +937,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1018,7 +960,7 @@
     </row>
     <row r="2" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>1</v>
@@ -1027,25 +969,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="9"/>
@@ -1060,7 +1002,7 @@
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1074,7 +1016,7 @@
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -1085,7 +1027,7 @@
     </row>
     <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -1096,7 +1038,7 @@
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1116,7 +1058,7 @@
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>1</v>
@@ -1125,28 +1067,28 @@
         <v>2</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="4"/>
@@ -1156,7 +1098,7 @@
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1165,7 +1107,7 @@
     </row>
     <row r="9" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1174,7 +1116,7 @@
     </row>
     <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -1183,7 +1125,7 @@
     </row>
     <row r="11" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -1192,7 +1134,7 @@
     </row>
     <row r="12" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -1201,7 +1143,7 @@
     </row>
     <row r="13" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1221,7 +1163,7 @@
     </row>
     <row r="14" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>1</v>
@@ -1230,28 +1172,28 @@
         <v>2</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="4"/>
@@ -1261,7 +1203,7 @@
     </row>
     <row r="15" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -1270,7 +1212,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1286,7 +1228,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1302,7 +1244,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1318,7 +1260,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1334,7 +1276,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1350,7 +1292,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>1</v>
@@ -1359,34 +1301,34 @@
         <v>2</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1402,7 +1344,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1418,7 +1360,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1434,7 +1376,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1450,7 +1392,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1466,7 +1408,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1482,7 +1424,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>1</v>
@@ -1491,34 +1433,34 @@
         <v>2</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L28" s="10"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1534,7 +1476,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1550,7 +1492,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1566,7 +1508,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1582,7 +1524,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1598,7 +1540,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1614,7 +1556,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>1</v>
@@ -1623,34 +1565,34 @@
         <v>2</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L35" s="10"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1666,7 +1608,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1682,7 +1624,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1698,7 +1640,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1714,7 +1656,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>

</xml_diff>